<commit_message>
conforming to Akoya nomenclature
</commit_message>
<xml_diff>
--- a/protocols/blue dye demo/labware layout.xlsx
+++ b/protocols/blue dye demo/labware layout.xlsx
@@ -12,226 +12,27 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
-    <t xml:space="preserve">Antibody plate (96-well plate, sealed with a pierceable sealing sheet, i.e. aluminum foil) </t>
+    <t>Deck position 1</t>
   </si>
   <si>
-    <t>Deck position 3</t>
+    <t>Buffers plate (Parhelia 12-trough)</t>
   </si>
   <si>
     <t>Volume</t>
   </si>
   <si>
-    <t>Preparation instructions</t>
-  </si>
-  <si>
-    <t>А</t>
-  </si>
-  <si>
-    <t>Preblock 1</t>
-  </si>
-  <si>
-    <t>Preblock 2</t>
-  </si>
-  <si>
-    <t>Preblock 3</t>
-  </si>
-  <si>
-    <t>Preblock 4</t>
-  </si>
-  <si>
-    <t>Preblock 5</t>
-  </si>
-  <si>
-    <t>Preblock 6</t>
-  </si>
-  <si>
-    <t>Preblock 7</t>
-  </si>
-  <si>
-    <t>Preblock 8</t>
-  </si>
-  <si>
-    <t>Preblock 9</t>
-  </si>
-  <si>
-    <t>Preblock 10</t>
-  </si>
-  <si>
-    <t>Preblock 11</t>
-  </si>
-  <si>
-    <t>Preblock 12</t>
-  </si>
-  <si>
-    <t>150ul</t>
-  </si>
-  <si>
-    <t>As per CODEX protocol</t>
-  </si>
-  <si>
     <t>A</t>
-  </si>
-  <si>
-    <t>Ab cocktail 1</t>
-  </si>
-  <si>
-    <t>Ab cocktail 2</t>
-  </si>
-  <si>
-    <t>Ab cocktail 3</t>
-  </si>
-  <si>
-    <t>Ab cocktail 4</t>
-  </si>
-  <si>
-    <t>Ab cocktail 5</t>
-  </si>
-  <si>
-    <t>Ab cocktail 6</t>
-  </si>
-  <si>
-    <t>Ab cocktail 7</t>
-  </si>
-  <si>
-    <t>Ab cocktail 8</t>
-  </si>
-  <si>
-    <t>Ab cocktail 9</t>
-  </si>
-  <si>
-    <t>Ab cocktail 10</t>
-  </si>
-  <si>
-    <t>Ab cocktail 11</t>
-  </si>
-  <si>
-    <t>Ab cocktail 12</t>
-  </si>
-  <si>
-    <t>C</t>
-  </si>
-  <si>
-    <t>BS3 in DMSO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">7ul </t>
-  </si>
-  <si>
-    <t>1 Aliquote of Reagent F (BS3) diluted in 50ul of dry DMSO</t>
-  </si>
-  <si>
-    <t>D</t>
-  </si>
-  <si>
-    <t>Rendering Mix 1</t>
-  </si>
-  <si>
-    <t>Rendering Mix 2</t>
-  </si>
-  <si>
-    <t>Rendering Mix 3</t>
-  </si>
-  <si>
-    <t>Rendering Mix 4</t>
-  </si>
-  <si>
-    <t>Rendering Mix 5</t>
-  </si>
-  <si>
-    <t>Rendering Mix 6</t>
-  </si>
-  <si>
-    <t>Rendering Mix 7</t>
-  </si>
-  <si>
-    <t>Rendering Mix 8</t>
-  </si>
-  <si>
-    <t>Rendering Mix 9</t>
-  </si>
-  <si>
-    <t>Rendering Mix 10</t>
-  </si>
-  <si>
-    <t>Rendering Mix 11</t>
-  </si>
-  <si>
-    <t>Rendering Mix 12</t>
-  </si>
-  <si>
-    <t>detector oligo mix in 150ul of R1 with BC3</t>
-  </si>
-  <si>
-    <t>E</t>
-  </si>
-  <si>
-    <t>F</t>
-  </si>
-  <si>
-    <t>G</t>
-  </si>
-  <si>
-    <t>H</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Buffers plate (12-trough, sealed with a pierceable sealing sheet, i.e. aluminum foil) </t>
-  </si>
-  <si>
-    <t>Deck position 1</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-      </rPr>
-      <t xml:space="preserve">1.6% PFA S1 </t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <b/>
-        <color rgb="FFFF0000"/>
-        <sz val="12.0"/>
-      </rPr>
-      <t>(no conditioner</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <color theme="1"/>
-      </rPr>
-      <t>)</t>
-    </r>
-  </si>
-  <si>
-    <t>S2</t>
-  </si>
-  <si>
-    <t>4% PFA in S4</t>
-  </si>
-  <si>
-    <t>MeOH</t>
   </si>
   <si>
     <t>PBS</t>
   </si>
   <si>
-    <t>H2</t>
+    <t>PBS + 0.1% Trypan blue</t>
   </si>
   <si>
-    <t>Pink (hybridization)</t>
-  </si>
-  <si>
-    <t>Blue (stripping)</t>
-  </si>
-  <si>
-    <t>Storage</t>
-  </si>
-  <si>
-    <t>20 ml</t>
+    <t>5 ml</t>
   </si>
 </sst>
 </file>
@@ -255,7 +56,7 @@
     </font>
     <font/>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -268,23 +69,15 @@
         <bgColor rgb="FFEFEFEF"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="5">
+  <borders count="4">
     <border/>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-    </border>
     <border>
       <left style="thin">
         <color rgb="FF000000"/>
@@ -319,40 +112,36 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="13">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" wrapText="0"/>
+      <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="1" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" vertical="center"/>
+    </xf>
+    <xf borderId="2" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="3" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf borderId="2" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="2" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="2" fillId="0" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf borderId="3" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="4" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -588,23 +377,12 @@
       <c r="G1" s="1"/>
     </row>
     <row r="2" ht="15.75" customHeight="1">
-      <c r="A2" s="1"/>
       <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="3" t="s">
+      <c r="C2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
-      <c r="K2" s="1"/>
-      <c r="L2" s="1"/>
-      <c r="M2" s="1"/>
     </row>
     <row r="3" ht="15.75" customHeight="1">
       <c r="B3" s="4">
@@ -643,429 +421,150 @@
       <c r="M3" s="1">
         <v>12.0</v>
       </c>
-      <c r="N3" s="3" t="s">
+      <c r="N3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="O3" s="3" t="s">
-        <v>3</v>
-      </c>
+      <c r="O3" s="2"/>
     </row>
     <row r="4" ht="15.75" customHeight="1">
       <c r="A4" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="C4" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="7"/>
+      <c r="H4" s="7"/>
+      <c r="I4" s="7"/>
+      <c r="J4" s="7"/>
+      <c r="K4" s="8"/>
+      <c r="L4" s="8"/>
+      <c r="M4" s="8"/>
+      <c r="N4" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="E4" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="F4" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="G4" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="H4" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="I4" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="J4" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="K4" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="L4" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="M4" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="N4" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="O4" s="4" t="s">
-        <v>18</v>
-      </c>
+      <c r="O4" s="4"/>
     </row>
     <row r="5" ht="15.75" customHeight="1">
-      <c r="A5" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="E5" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="F5" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="G5" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="H5" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="I5" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="J5" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="K5" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="L5" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="M5" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="N5" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="O5" s="4" t="s">
-        <v>18</v>
-      </c>
+      <c r="B5" s="10"/>
+      <c r="C5" s="10"/>
+      <c r="D5" s="10"/>
+      <c r="E5" s="10"/>
+      <c r="F5" s="10"/>
+      <c r="G5" s="10"/>
+      <c r="H5" s="10"/>
+      <c r="I5" s="10"/>
+      <c r="J5" s="10"/>
+      <c r="K5" s="10"/>
+      <c r="L5" s="10"/>
+      <c r="M5" s="10"/>
+      <c r="O5" s="4"/>
     </row>
     <row r="6" ht="15.75" customHeight="1">
-      <c r="A6" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="D6" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="E6" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="F6" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="G6" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="H6" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="I6" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="J6" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="K6" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="L6" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="M6" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="N6" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="O6" s="4" t="s">
-        <v>35</v>
-      </c>
+      <c r="B6" s="10"/>
+      <c r="C6" s="10"/>
+      <c r="D6" s="10"/>
+      <c r="E6" s="10"/>
+      <c r="F6" s="10"/>
+      <c r="G6" s="10"/>
+      <c r="H6" s="10"/>
+      <c r="I6" s="10"/>
+      <c r="J6" s="10"/>
+      <c r="K6" s="10"/>
+      <c r="L6" s="10"/>
+      <c r="M6" s="10"/>
+      <c r="O6" s="4"/>
     </row>
     <row r="7" ht="15.75" customHeight="1">
-      <c r="A7" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="E7" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="F7" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="G7" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="H7" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="I7" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="J7" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="K7" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="L7" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="M7" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="N7" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="O7" s="4" t="s">
-        <v>49</v>
-      </c>
+      <c r="B7" s="10"/>
+      <c r="C7" s="10"/>
+      <c r="D7" s="10"/>
+      <c r="E7" s="10"/>
+      <c r="F7" s="10"/>
+      <c r="G7" s="10"/>
+      <c r="H7" s="10"/>
+      <c r="I7" s="10"/>
+      <c r="J7" s="10"/>
+      <c r="K7" s="10"/>
+      <c r="L7" s="10"/>
+      <c r="M7" s="10"/>
+      <c r="O7" s="4"/>
     </row>
     <row r="8" ht="15.75" customHeight="1">
-      <c r="A8" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="B8" s="6"/>
-      <c r="C8" s="7"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="7"/>
-      <c r="F8" s="6"/>
-      <c r="G8" s="7"/>
-      <c r="H8" s="7"/>
-      <c r="I8" s="7"/>
-      <c r="J8" s="7"/>
-      <c r="K8" s="7"/>
-      <c r="L8" s="7"/>
-      <c r="M8" s="7"/>
+      <c r="B8" s="10"/>
+      <c r="C8" s="10"/>
+      <c r="D8" s="10"/>
+      <c r="E8" s="10"/>
+      <c r="F8" s="10"/>
+      <c r="G8" s="10"/>
+      <c r="H8" s="10"/>
+      <c r="I8" s="10"/>
+      <c r="J8" s="10"/>
+      <c r="K8" s="10"/>
+      <c r="L8" s="10"/>
+      <c r="M8" s="10"/>
     </row>
     <row r="9" ht="15.75" customHeight="1">
-      <c r="A9" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="B9" s="6"/>
-      <c r="C9" s="7"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="7"/>
-      <c r="F9" s="6"/>
-      <c r="G9" s="7"/>
-      <c r="H9" s="7"/>
-      <c r="I9" s="7"/>
-      <c r="J9" s="7"/>
-      <c r="K9" s="7"/>
-      <c r="L9" s="7"/>
-      <c r="M9" s="7"/>
+      <c r="B9" s="11"/>
+      <c r="C9" s="11"/>
+      <c r="D9" s="11"/>
+      <c r="E9" s="11"/>
+      <c r="F9" s="11"/>
+      <c r="G9" s="11"/>
+      <c r="H9" s="11"/>
+      <c r="I9" s="11"/>
+      <c r="J9" s="11"/>
+      <c r="K9" s="11"/>
+      <c r="L9" s="11"/>
+      <c r="M9" s="11"/>
     </row>
     <row r="10" ht="15.75" customHeight="1">
-      <c r="A10" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="B10" s="6"/>
-      <c r="C10" s="7"/>
-      <c r="D10" s="6"/>
-      <c r="E10" s="7"/>
-      <c r="F10" s="6"/>
-      <c r="G10" s="7"/>
-      <c r="H10" s="7"/>
-      <c r="I10" s="7"/>
-      <c r="J10" s="7"/>
-      <c r="K10" s="7"/>
-      <c r="L10" s="7"/>
-      <c r="M10" s="7"/>
+      <c r="A10" s="12"/>
+      <c r="B10" s="1"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="4"/>
+      <c r="H10" s="4"/>
+      <c r="I10" s="4"/>
+      <c r="J10" s="4"/>
+      <c r="K10" s="4"/>
+      <c r="L10" s="4"/>
+      <c r="M10" s="4"/>
     </row>
     <row r="11" ht="15.75" customHeight="1">
-      <c r="A11" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="B11" s="6"/>
-      <c r="C11" s="7"/>
-      <c r="D11" s="6"/>
-      <c r="E11" s="7"/>
-      <c r="F11" s="6"/>
-      <c r="G11" s="7"/>
-      <c r="H11" s="7"/>
-      <c r="I11" s="7"/>
-      <c r="J11" s="7"/>
-      <c r="K11" s="7"/>
-      <c r="L11" s="7"/>
-      <c r="M11" s="7"/>
+      <c r="A11" s="12"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="4"/>
+      <c r="H11" s="4"/>
+      <c r="I11" s="4"/>
+      <c r="J11" s="4"/>
+      <c r="K11" s="4"/>
+      <c r="L11" s="4"/>
+      <c r="M11" s="4"/>
     </row>
     <row r="12" ht="15.75" customHeight="1">
       <c r="B12" s="1"/>
     </row>
-    <row r="13" ht="15.75" customHeight="1">
-      <c r="B13" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="H13" s="3" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="14" ht="15.75" customHeight="1">
-      <c r="B14" s="4">
-        <v>1.0</v>
-      </c>
-      <c r="C14" s="4">
-        <v>2.0</v>
-      </c>
-      <c r="D14" s="4">
-        <v>3.0</v>
-      </c>
-      <c r="E14" s="4">
-        <v>4.0</v>
-      </c>
-      <c r="F14" s="4">
-        <v>5.0</v>
-      </c>
-      <c r="G14" s="4">
-        <v>6.0</v>
-      </c>
-      <c r="H14" s="1">
-        <v>7.0</v>
-      </c>
-      <c r="I14" s="1">
-        <v>8.0</v>
-      </c>
-      <c r="J14" s="1">
-        <v>9.0</v>
-      </c>
-      <c r="K14" s="1">
-        <v>10.0</v>
-      </c>
-      <c r="L14" s="1">
-        <v>11.0</v>
-      </c>
-      <c r="M14" s="1">
-        <v>12.0</v>
-      </c>
-      <c r="N14" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="15" ht="15.75" customHeight="1">
-      <c r="A15" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="B15" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="C15" s="10" t="s">
-        <v>57</v>
-      </c>
-      <c r="D15" s="10" t="s">
-        <v>58</v>
-      </c>
-      <c r="E15" s="10" t="s">
-        <v>59</v>
-      </c>
-      <c r="F15" s="10" t="s">
-        <v>60</v>
-      </c>
-      <c r="G15" s="10" t="s">
-        <v>61</v>
-      </c>
-      <c r="H15" s="10" t="s">
-        <v>62</v>
-      </c>
-      <c r="I15" s="10" t="s">
-        <v>63</v>
-      </c>
-      <c r="J15" s="9" t="s">
-        <v>64</v>
-      </c>
-      <c r="K15" s="11"/>
-      <c r="L15" s="11"/>
-      <c r="M15" s="11"/>
-      <c r="N15" s="12" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="16" ht="15.75" customHeight="1">
-      <c r="B16" s="13"/>
-      <c r="C16" s="13"/>
-      <c r="D16" s="13"/>
-      <c r="E16" s="13"/>
-      <c r="F16" s="13"/>
-      <c r="G16" s="13"/>
-      <c r="H16" s="13"/>
-      <c r="I16" s="13"/>
-      <c r="J16" s="13"/>
-      <c r="K16" s="13"/>
-      <c r="L16" s="13"/>
-      <c r="M16" s="13"/>
-    </row>
-    <row r="17" ht="15.75" customHeight="1">
-      <c r="B17" s="13"/>
-      <c r="C17" s="13"/>
-      <c r="D17" s="13"/>
-      <c r="E17" s="13"/>
-      <c r="F17" s="13"/>
-      <c r="G17" s="13"/>
-      <c r="H17" s="13"/>
-      <c r="I17" s="13"/>
-      <c r="J17" s="13"/>
-      <c r="K17" s="13"/>
-      <c r="L17" s="13"/>
-      <c r="M17" s="13"/>
-    </row>
-    <row r="18" ht="15.75" customHeight="1">
-      <c r="B18" s="13"/>
-      <c r="C18" s="13"/>
-      <c r="D18" s="13"/>
-      <c r="E18" s="13"/>
-      <c r="F18" s="13"/>
-      <c r="G18" s="13"/>
-      <c r="H18" s="13"/>
-      <c r="I18" s="13"/>
-      <c r="J18" s="13"/>
-      <c r="K18" s="13"/>
-      <c r="L18" s="13"/>
-      <c r="M18" s="13"/>
-    </row>
-    <row r="19" ht="15.75" customHeight="1">
-      <c r="B19" s="13"/>
-      <c r="C19" s="13"/>
-      <c r="D19" s="13"/>
-      <c r="E19" s="13"/>
-      <c r="F19" s="13"/>
-      <c r="G19" s="13"/>
-      <c r="H19" s="13"/>
-      <c r="I19" s="13"/>
-      <c r="J19" s="13"/>
-      <c r="K19" s="13"/>
-      <c r="L19" s="13"/>
-      <c r="M19" s="13"/>
-    </row>
-    <row r="20" ht="15.75" customHeight="1">
-      <c r="B20" s="14"/>
-      <c r="C20" s="14"/>
-      <c r="D20" s="14"/>
-      <c r="E20" s="14"/>
-      <c r="F20" s="14"/>
-      <c r="G20" s="14"/>
-      <c r="H20" s="14"/>
-      <c r="I20" s="14"/>
-      <c r="J20" s="14"/>
-      <c r="K20" s="14"/>
-      <c r="L20" s="14"/>
-      <c r="M20" s="14"/>
-    </row>
+    <row r="13" ht="15.75" customHeight="1"/>
+    <row r="14" ht="15.75" customHeight="1"/>
+    <row r="15" ht="15.75" customHeight="1"/>
+    <row r="16" ht="15.75" customHeight="1"/>
+    <row r="17" ht="15.75" customHeight="1"/>
+    <row r="18" ht="15.75" customHeight="1"/>
+    <row r="19" ht="15.75" customHeight="1"/>
+    <row r="20" ht="15.75" customHeight="1"/>
     <row r="21" ht="15.75" customHeight="1"/>
     <row r="22" ht="15.75" customHeight="1"/>
     <row r="23" ht="15.75" customHeight="1"/>
@@ -2032,22 +1531,36 @@
     <row r="984" ht="15.75" customHeight="1"/>
     <row r="985" ht="15.75" customHeight="1"/>
     <row r="986" ht="15.75" customHeight="1"/>
+    <row r="987" ht="15.75" customHeight="1"/>
+    <row r="988" ht="15.75" customHeight="1"/>
+    <row r="989" ht="15.75" customHeight="1"/>
+    <row r="990" ht="15.75" customHeight="1"/>
+    <row r="991" ht="15.75" customHeight="1"/>
+    <row r="992" ht="15.75" customHeight="1"/>
+    <row r="993" ht="15.75" customHeight="1"/>
+    <row r="994" ht="15.75" customHeight="1"/>
+    <row r="995" ht="15.75" customHeight="1"/>
+    <row r="996" ht="15.75" customHeight="1"/>
+    <row r="997" ht="15.75" customHeight="1"/>
+    <row r="998" ht="15.75" customHeight="1"/>
+    <row r="999" ht="15.75" customHeight="1"/>
+    <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="N15:N20"/>
-    <mergeCell ref="M15:M20"/>
-    <mergeCell ref="A15:A20"/>
-    <mergeCell ref="D15:D20"/>
-    <mergeCell ref="C15:C20"/>
-    <mergeCell ref="B15:B20"/>
-    <mergeCell ref="E15:E20"/>
-    <mergeCell ref="L15:L20"/>
-    <mergeCell ref="G15:G20"/>
-    <mergeCell ref="H15:H20"/>
-    <mergeCell ref="I15:I20"/>
-    <mergeCell ref="J15:J20"/>
-    <mergeCell ref="K15:K20"/>
-    <mergeCell ref="F15:F20"/>
+    <mergeCell ref="A4:A9"/>
+    <mergeCell ref="B4:B9"/>
+    <mergeCell ref="C4:C9"/>
+    <mergeCell ref="D4:D9"/>
+    <mergeCell ref="E4:E9"/>
+    <mergeCell ref="F4:F9"/>
+    <mergeCell ref="H4:H9"/>
+    <mergeCell ref="I4:I9"/>
+    <mergeCell ref="J4:J9"/>
+    <mergeCell ref="K4:K9"/>
+    <mergeCell ref="L4:L9"/>
+    <mergeCell ref="M4:M9"/>
+    <mergeCell ref="N4:N9"/>
+    <mergeCell ref="G4:G9"/>
   </mergeCells>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>